<commit_message>
added support for ternary diagramms
</commit_message>
<xml_diff>
--- a/ExcelSheet/Werte.xlsx
+++ b/ExcelSheet/Werte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Projects\cuteTHiepy\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FF5045-E6CD-43C7-81CB-990F4A468DED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90203766-75C1-4566-832A-C8F1E48F3B79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7845" activeTab="1" xr2:uid="{126B0C31-9675-43AF-BAED-15DFE472465D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7845" xr2:uid="{964F1E2F-A1A8-4B1B-8A20-7F72E68070CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
   <si>
     <t>x axis / -</t>
   </si>
@@ -46,23 +55,18 @@
     <t>f1</t>
   </si>
   <si>
-    <t>ok</t>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>-k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,7 +96,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -406,94 +410,353 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D3C11D-0332-4630-9D6F-6A143DF040AC}">
-  <dimension ref="A2:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527C3474-F86F-4CBC-90D2-543534C56B37}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>0.19153000000000001</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.17688999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.63158000000000003</v>
+      </c>
+      <c r="D2">
+        <v>0.14960999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.20588999999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.64449000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>0.27531</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.13522000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.58947000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.1032</v>
+      </c>
+      <c r="E3">
+        <v>0.25320999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0.64358000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>0.33872000000000002</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0.11391</v>
+      </c>
+      <c r="C4">
+        <v>0.54737000000000002</v>
+      </c>
+      <c r="D4">
+        <v>7.1669999999999998E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.30081999999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.62751000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>0.39555000000000001</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>9.919E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.50526000000000004</v>
+      </c>
+      <c r="D5">
+        <v>5.0889999999999998E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.34617999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.60292999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>0.44880999999999999</v>
       </c>
       <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>8.8029999999999997E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.46316000000000002</v>
+      </c>
+      <c r="D6">
+        <v>3.6269999999999997E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.39137</v>
+      </c>
+      <c r="F6">
+        <v>0.57235999999999998</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>0.49980999999999998</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>7.9140000000000002E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.42104999999999998</v>
+      </c>
+      <c r="D7">
+        <v>2.572E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.43741000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.53686999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>0.54923</v>
       </c>
       <c r="B8">
-        <v>36</v>
+        <v>7.1819999999999995E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.37895000000000001</v>
+      </c>
+      <c r="D8">
+        <v>1.805E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.48493999999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.49701000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>0.59750000000000003</v>
       </c>
       <c r="B9">
-        <v>49</v>
+        <v>6.5659999999999996E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.33683999999999997</v>
+      </c>
+      <c r="D9">
+        <v>1.251E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.53444000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.45305000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>0.64488000000000001</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>6.0380000000000003E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.29474</v>
+      </c>
+      <c r="D10">
+        <v>8.5299999999999994E-3</v>
+      </c>
+      <c r="E10">
+        <v>0.58630000000000004</v>
+      </c>
+      <c r="F10">
+        <v>0.40516999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>0.69157000000000002</v>
       </c>
       <c r="B11">
-        <v>81</v>
+        <v>5.5800000000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.25263000000000002</v>
+      </c>
+      <c r="D11">
+        <v>5.7200000000000003E-3</v>
+      </c>
+      <c r="E11">
+        <v>0.64080000000000004</v>
+      </c>
+      <c r="F11">
+        <v>0.35348000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.73768999999999996</v>
+      </c>
+      <c r="B12">
+        <v>5.178E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.21052999999999999</v>
+      </c>
+      <c r="D12">
+        <v>3.7799999999999999E-3</v>
+      </c>
+      <c r="E12">
+        <v>0.69816</v>
+      </c>
+      <c r="F12">
+        <v>0.29805999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.78335999999999995</v>
+      </c>
+      <c r="B13">
+        <v>4.8219999999999999E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.16841999999999999</v>
+      </c>
+      <c r="D13">
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="E13">
+        <v>0.75851999999999997</v>
+      </c>
+      <c r="F13">
+        <v>0.29805999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.82865</v>
+      </c>
+      <c r="B14">
+        <v>4.5030000000000001E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.12631999999999999</v>
+      </c>
+      <c r="D14">
+        <v>1.57E-3</v>
+      </c>
+      <c r="E14">
+        <v>0.82191999999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.17651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.87361</v>
+      </c>
+      <c r="B15">
+        <v>4.2180000000000002E-2</v>
+      </c>
+      <c r="C15">
+        <v>8.4209999999999993E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.9852399999999998E-4</v>
+      </c>
+      <c r="E15">
+        <v>0.88827999999999996</v>
+      </c>
+      <c r="F15">
+        <v>0.11072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="B16">
+        <v>3.959E-2</v>
+      </c>
+      <c r="C16">
+        <v>4.2110000000000002E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.2920599999999999E-4</v>
+      </c>
+      <c r="E16">
+        <v>0.95737000000000005</v>
+      </c>
+      <c r="F16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.96272999999999997</v>
+      </c>
+      <c r="B17">
+        <v>3.7269999999999998E-2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.2781100000000001E-7</v>
+      </c>
+      <c r="E17">
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.6079699999999999E-5</v>
       </c>
     </row>
   </sheetData>
@@ -502,182 +765,477 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5B39B6-0F04-4C08-B6C3-ED9ECE3BD682}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA98769-166D-43A3-B25C-04B17C8AFC57}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>Tabelle1!$A$2/$A$14</f>
-        <v>0</v>
+        <f>Tabelle1!$A$2</f>
+        <v>0.19153000000000001</v>
       </c>
       <c r="B5">
         <f>Tabelle1!$B$2</f>
-        <v>0</v>
+        <v>0.17688999999999999</v>
       </c>
       <c r="C5">
-        <f>Tabelle1!$A$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$2</f>
+        <v>0.63158000000000003</v>
+      </c>
+      <c r="D5">
+        <f>Tabelle1!$D$2</f>
+        <v>0.14960999999999999</v>
+      </c>
+      <c r="E5">
+        <f>Tabelle1!$E$2</f>
+        <v>0.20588999999999999</v>
+      </c>
+      <c r="F5">
+        <f>Tabelle1!$F$2</f>
+        <v>0.64449000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>Tabelle1!$A$3</f>
-        <v>1</v>
+        <v>0.27531</v>
       </c>
       <c r="B6">
         <f>Tabelle1!$B$3</f>
-        <v>1</v>
+        <v>0.13522000000000001</v>
       </c>
       <c r="C6">
-        <f>Tabelle1!$A$3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$3</f>
+        <v>0.58947000000000005</v>
+      </c>
+      <c r="D6">
+        <f>Tabelle1!$D$3</f>
+        <v>0.1032</v>
+      </c>
+      <c r="E6">
+        <f>Tabelle1!$E$3</f>
+        <v>0.25320999999999999</v>
+      </c>
+      <c r="F6">
+        <f>Tabelle1!$F$3</f>
+        <v>0.64358000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>Tabelle1!$A$4</f>
-        <v>2</v>
+        <v>0.33872000000000002</v>
       </c>
       <c r="B7">
         <f>Tabelle1!$B$4</f>
-        <v>4</v>
+        <v>0.11391</v>
       </c>
       <c r="C7">
-        <f>Tabelle1!$A$4</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$4</f>
+        <v>0.54737000000000002</v>
+      </c>
+      <c r="D7">
+        <f>Tabelle1!$D$4</f>
+        <v>7.1669999999999998E-2</v>
+      </c>
+      <c r="E7">
+        <f>Tabelle1!$E$4</f>
+        <v>0.30081999999999998</v>
+      </c>
+      <c r="F7">
+        <f>Tabelle1!$F$4</f>
+        <v>0.62751000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>Tabelle1!$A$5</f>
-        <v>3</v>
+        <v>0.39555000000000001</v>
       </c>
       <c r="B8">
         <f>Tabelle1!$B$5</f>
-        <v>9</v>
+        <v>9.919E-2</v>
       </c>
       <c r="C8">
-        <f>Tabelle1!$A$5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$5</f>
+        <v>0.50526000000000004</v>
+      </c>
+      <c r="D8">
+        <f>Tabelle1!$D$5</f>
+        <v>5.0889999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <f>Tabelle1!$E$5</f>
+        <v>0.34617999999999999</v>
+      </c>
+      <c r="F8">
+        <f>Tabelle1!$F$5</f>
+        <v>0.60292999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>Tabelle1!$A$6</f>
-        <v>4</v>
+        <v>0.44880999999999999</v>
       </c>
       <c r="B9">
         <f>Tabelle1!$B$6</f>
-        <v>16</v>
+        <v>8.8029999999999997E-2</v>
       </c>
       <c r="C9">
-        <f>Tabelle1!$A$6</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$6</f>
+        <v>0.46316000000000002</v>
+      </c>
+      <c r="D9">
+        <f>Tabelle1!$D$6</f>
+        <v>3.6269999999999997E-2</v>
+      </c>
+      <c r="E9">
+        <f>Tabelle1!$E$6</f>
+        <v>0.39137</v>
+      </c>
+      <c r="F9">
+        <f>Tabelle1!$F$6</f>
+        <v>0.57235999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>Tabelle1!$A$7</f>
-        <v>5</v>
+        <v>0.49980999999999998</v>
       </c>
       <c r="B10">
         <f>Tabelle1!$B$7</f>
-        <v>25</v>
+        <v>7.9140000000000002E-2</v>
       </c>
       <c r="C10">
-        <f>Tabelle1!$A$7</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$7</f>
+        <v>0.42104999999999998</v>
+      </c>
+      <c r="D10">
+        <f>Tabelle1!$D$7</f>
+        <v>2.572E-2</v>
+      </c>
+      <c r="E10">
+        <f>Tabelle1!$E$7</f>
+        <v>0.43741000000000002</v>
+      </c>
+      <c r="F10">
+        <f>Tabelle1!$F$7</f>
+        <v>0.53686999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>Tabelle1!$A$8</f>
-        <v>6</v>
+        <v>0.54923</v>
       </c>
       <c r="B11">
         <f>Tabelle1!$B$8</f>
-        <v>36</v>
+        <v>7.1819999999999995E-2</v>
       </c>
       <c r="C11">
-        <f>Tabelle1!$A$8</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$8</f>
+        <v>0.37895000000000001</v>
+      </c>
+      <c r="D11">
+        <f>Tabelle1!$D$8</f>
+        <v>1.805E-2</v>
+      </c>
+      <c r="E11">
+        <f>Tabelle1!$E$8</f>
+        <v>0.48493999999999998</v>
+      </c>
+      <c r="F11">
+        <f>Tabelle1!$F$8</f>
+        <v>0.49701000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>Tabelle1!$A$9</f>
-        <v>7</v>
+        <v>0.59750000000000003</v>
       </c>
       <c r="B12">
         <f>Tabelle1!$B$9</f>
-        <v>49</v>
+        <v>6.5659999999999996E-2</v>
       </c>
       <c r="C12">
-        <f>Tabelle1!$A$9</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$9</f>
+        <v>0.33683999999999997</v>
+      </c>
+      <c r="D12">
+        <f>Tabelle1!$D$9</f>
+        <v>1.251E-2</v>
+      </c>
+      <c r="E12">
+        <f>Tabelle1!$E$9</f>
+        <v>0.53444000000000003</v>
+      </c>
+      <c r="F12">
+        <f>Tabelle1!$F$9</f>
+        <v>0.45305000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>Tabelle1!$A$10</f>
-        <v>8</v>
+        <v>0.64488000000000001</v>
       </c>
       <c r="B13">
         <f>Tabelle1!$B$10</f>
-        <v>64</v>
+        <v>6.0380000000000003E-2</v>
       </c>
       <c r="C13">
-        <f>Tabelle1!$A$10</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Tabelle1!$C$10</f>
+        <v>0.29474</v>
+      </c>
+      <c r="D13">
+        <f>Tabelle1!$D$10</f>
+        <v>8.5299999999999994E-3</v>
+      </c>
+      <c r="E13">
+        <f>Tabelle1!$E$10</f>
+        <v>0.58630000000000004</v>
+      </c>
+      <c r="F13">
+        <f>Tabelle1!$F$10</f>
+        <v>0.40516999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>Tabelle1!$A$11</f>
-        <v>9</v>
+        <v>0.69157000000000002</v>
       </c>
       <c r="B14">
         <f>Tabelle1!$B$11</f>
-        <v>81</v>
+        <v>5.5800000000000002E-2</v>
       </c>
       <c r="C14">
-        <f>Tabelle1!$A$11</f>
-        <v>9</v>
+        <f>Tabelle1!$C$11</f>
+        <v>0.25263000000000002</v>
+      </c>
+      <c r="D14">
+        <f>Tabelle1!$D$11</f>
+        <v>5.7200000000000003E-3</v>
+      </c>
+      <c r="E14">
+        <f>Tabelle1!$E$11</f>
+        <v>0.64080000000000004</v>
+      </c>
+      <c r="F14">
+        <f>Tabelle1!$F$11</f>
+        <v>0.35348000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>Tabelle1!$A$12</f>
+        <v>0.73768999999999996</v>
+      </c>
+      <c r="B15">
+        <f>Tabelle1!$B$12</f>
+        <v>5.178E-2</v>
+      </c>
+      <c r="C15">
+        <f>Tabelle1!$C$12</f>
+        <v>0.21052999999999999</v>
+      </c>
+      <c r="D15">
+        <f>Tabelle1!$D$12</f>
+        <v>3.7799999999999999E-3</v>
+      </c>
+      <c r="E15">
+        <f>Tabelle1!$E$12</f>
+        <v>0.69816</v>
+      </c>
+      <c r="F15">
+        <f>Tabelle1!$F$12</f>
+        <v>0.29805999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>Tabelle1!$A$13</f>
+        <v>0.78335999999999995</v>
+      </c>
+      <c r="B16">
+        <f>Tabelle1!$B$13</f>
+        <v>4.8219999999999999E-2</v>
+      </c>
+      <c r="C16">
+        <f>Tabelle1!$C$13</f>
+        <v>0.16841999999999999</v>
+      </c>
+      <c r="D16">
+        <f>Tabelle1!$D$13</f>
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="E16">
+        <f>Tabelle1!$E$13</f>
+        <v>0.75851999999999997</v>
+      </c>
+      <c r="F16">
+        <f>Tabelle1!$F$13</f>
+        <v>0.29805999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>Tabelle1!$A$14</f>
+        <v>0.82865</v>
+      </c>
+      <c r="B17">
+        <f>Tabelle1!$B$14</f>
+        <v>4.5030000000000001E-2</v>
+      </c>
+      <c r="C17">
+        <f>Tabelle1!$C$14</f>
+        <v>0.12631999999999999</v>
+      </c>
+      <c r="D17">
+        <f>Tabelle1!$D$14</f>
+        <v>1.57E-3</v>
+      </c>
+      <c r="E17">
+        <f>Tabelle1!$E$14</f>
+        <v>0.82191999999999998</v>
+      </c>
+      <c r="F17">
+        <f>Tabelle1!$F$14</f>
+        <v>0.17651</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>Tabelle1!$A$15</f>
+        <v>0.87361</v>
+      </c>
+      <c r="B18">
+        <f>Tabelle1!$B$15</f>
+        <v>4.2180000000000002E-2</v>
+      </c>
+      <c r="C18">
+        <f>Tabelle1!$C$15</f>
+        <v>8.4209999999999993E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f>Tabelle1!$D$15</f>
+        <v>9.9852399999999998E-4</v>
+      </c>
+      <c r="E18">
+        <f>Tabelle1!$E$15</f>
+        <v>0.88827999999999996</v>
+      </c>
+      <c r="F18">
+        <f>Tabelle1!$F$15</f>
+        <v>0.11072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>Tabelle1!$A$16</f>
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="B19">
+        <f>Tabelle1!$B$16</f>
+        <v>3.959E-2</v>
+      </c>
+      <c r="C19">
+        <f>Tabelle1!$C$16</f>
+        <v>4.2110000000000002E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <f>Tabelle1!$D$16</f>
+        <v>6.2920599999999999E-4</v>
+      </c>
+      <c r="E19">
+        <f>Tabelle1!$E$16</f>
+        <v>0.95737000000000005</v>
+      </c>
+      <c r="F19">
+        <f>Tabelle1!$F$16</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>Tabelle1!$A$17</f>
+        <v>0.96272999999999997</v>
+      </c>
+      <c r="B20">
+        <f>Tabelle1!$B$17</f>
+        <v>3.7269999999999998E-2</v>
+      </c>
+      <c r="C20">
+        <f>Tabelle1!$C$17</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <f>Tabelle1!$D$17</f>
+        <v>1.2781100000000001E-7</v>
+      </c>
+      <c r="E20">
+        <f>Tabelle1!$E$17</f>
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="F20" s="1">
+        <f>Tabelle1!$F$17</f>
+        <v>3.6079699999999999E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>Tabelle1!$B$18</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added common colors that replace the shorthand colors from matplotlib
</commit_message>
<xml_diff>
--- a/ExcelSheet/Werte.xlsx
+++ b/ExcelSheet/Werte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Projects\cuteTHiepy\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90203766-75C1-4566-832A-C8F1E48F3B79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF511DA-EB35-4DCA-B761-E603CF80DABD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7845" xr2:uid="{964F1E2F-A1A8-4B1B-8A20-7F72E68070CD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7845" activeTab="1" xr2:uid="{964F1E2F-A1A8-4B1B-8A20-7F72E68070CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>f2</t>
   </si>
   <si>
-    <t>-k</t>
+    <t>mo</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527C3474-F86F-4CBC-90D2-543534C56B37}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -766,9 +766,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA98769-166D-43A3-B25C-04B17C8AFC57}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1232,12 +1234,6 @@
         <v>3.6079699999999999E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f>Tabelle1!$B$18</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>